<commit_message>
change updated_dt, created_dt to updated_at, created_at, add field login_hash, last_login, group to table user
</commit_message>
<xml_diff>
--- a/doc/detail_design/db/MiniBlog_Database_Design.xlsx
+++ b/doc/detail_design/db/MiniBlog_Database_Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="259">
   <si>
     <t>No</t>
   </si>
@@ -783,30 +783,14 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>created_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Date User Update</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>updated_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Date Created</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>created_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>updated_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Post</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -851,22 +835,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>created_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>updated_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>created_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>updated_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>content</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -899,14 +867,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>created_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>updated_dt</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>username, firstname, lastname</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -940,6 +900,98 @@
   </si>
   <si>
     <t>No</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>created_at</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>updated_at</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Group</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>INT(11)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Last Login</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>last_login</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>569976899766</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Login Hash</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>login_hash</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Token: xxxxxxxxx</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>09018238123</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>j123@afsj@aff</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>updated_at</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>created_at</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>created_at</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>updated_at</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3438,7 +3490,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3893,26 +3945,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3920,12 +3972,6 @@
     <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3962,20 +4008,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4030,6 +4082,21 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="462">
@@ -7323,7 +7390,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="123" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C4" s="137" t="str">
         <f>HYPERLINK("#post","post")</f>
@@ -7554,10 +7621,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -7576,117 +7643,117 @@
     <col min="16" max="16" width="17" style="13" customWidth="1"/>
     <col min="17" max="17" width="15.5" style="13" customWidth="1"/>
     <col min="18" max="19" width="8.83203125" style="13"/>
-    <col min="20" max="20" width="14" style="13" customWidth="1"/>
-    <col min="21" max="22" width="13.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.83203125" style="13"/>
+    <col min="20" max="23" width="14" style="13" customWidth="1"/>
+    <col min="24" max="25" width="13.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="12" thickBot="1">
+    <row r="1" spans="1:25" ht="12" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="13">
+    <row r="2" spans="1:25" ht="13">
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="187" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="167"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="166"/>
-      <c r="G2" s="170"/>
-    </row>
-    <row r="3" spans="1:22" ht="13">
+      <c r="F2" s="187"/>
+      <c r="G2" s="188"/>
+    </row>
+    <row r="3" spans="1:25" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="169"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="189" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="172"/>
-    </row>
-    <row r="4" spans="1:22" ht="13">
+      <c r="G3" s="190"/>
+    </row>
+    <row r="4" spans="1:25" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="191" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="172"/>
-    </row>
-    <row r="5" spans="1:22" ht="13">
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
+    </row>
+    <row r="5" spans="1:25" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="191" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="169"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="172"/>
-    </row>
-    <row r="6" spans="1:22" ht="13">
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
+    </row>
+    <row r="6" spans="1:25" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="168" t="s">
+      <c r="C6" s="191" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="169"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="172"/>
-    </row>
-    <row r="7" spans="1:22" ht="13">
-      <c r="B7" s="177" t="s">
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
+    </row>
+    <row r="7" spans="1:25" ht="13">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="179"/>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="B8" s="180"/>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="182"/>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="B9" s="183"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="182"/>
-    </row>
-    <row r="10" spans="1:22" ht="12" thickBot="1">
-      <c r="B10" s="184"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="186"/>
-    </row>
-    <row r="12" spans="1:22" ht="12" thickBot="1">
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
+    </row>
+    <row r="10" spans="1:25" ht="12" thickBot="1">
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
+    </row>
+    <row r="12" spans="1:25" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -7694,7 +7761,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:25">
       <c r="A13" s="30" t="s">
         <v>0</v>
       </c>
@@ -7753,13 +7820,22 @@
         <v>184</v>
       </c>
       <c r="U13" s="128" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="V13" s="128" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="17">
+        <v>244</v>
+      </c>
+      <c r="W13" s="128" t="s">
+        <v>248</v>
+      </c>
+      <c r="X13" s="128" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y13" s="128" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="17">
       <c r="A14" s="69">
         <v>1</v>
       </c>
@@ -7816,14 +7892,23 @@
       <c r="T14" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="U14" s="127">
+      <c r="U14" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="V14" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="W14" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="X14" s="127">
         <v>41996.702777777777</v>
       </c>
-      <c r="V14" s="127">
+      <c r="Y14" s="127">
         <v>41996.702777777777</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="17">
+    <row r="15" spans="1:25" ht="17">
       <c r="A15" s="59">
         <f>A14+1</f>
         <v>2</v>
@@ -7849,7 +7934,7 @@
       <c r="P15" s="127"/>
       <c r="Q15" s="127"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:25">
       <c r="A16" s="59">
         <f t="shared" ref="A16:A21" si="0">A15+1</f>
         <v>3</v>
@@ -8064,148 +8149,187 @@
       <c r="A26" s="69">
         <v>13</v>
       </c>
-      <c r="B26" s="147" t="s">
+      <c r="B26" s="212" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="213" t="s">
+        <v>238</v>
+      </c>
+      <c r="D26" s="213" t="s">
+        <v>240</v>
+      </c>
+      <c r="E26" s="214" t="s">
+        <v>241</v>
+      </c>
+      <c r="F26" s="215"/>
+      <c r="G26" s="216" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="69">
+        <v>14</v>
+      </c>
+      <c r="B27" s="212" t="s">
+        <v>243</v>
+      </c>
+      <c r="C27" s="213" t="s">
+        <v>244</v>
+      </c>
+      <c r="D27" s="213" t="s">
+        <v>240</v>
+      </c>
+      <c r="E27" s="214" t="s">
+        <v>245</v>
+      </c>
+      <c r="F27" s="215"/>
+      <c r="G27" s="216" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="69">
+        <v>15</v>
+      </c>
+      <c r="B28" s="212" t="s">
+        <v>247</v>
+      </c>
+      <c r="C28" s="213" t="s">
+        <v>248</v>
+      </c>
+      <c r="D28" s="213" t="s">
+        <v>249</v>
+      </c>
+      <c r="E28" s="214" t="s">
+        <v>245</v>
+      </c>
+      <c r="F28" s="215"/>
+      <c r="G28" s="216" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="69">
+        <v>16</v>
+      </c>
+      <c r="B29" s="147" t="s">
         <v>205</v>
       </c>
-      <c r="C26" s="148" t="s">
+      <c r="C29" s="148" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29" s="148" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="149" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="150"/>
+      <c r="G29" s="151" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12" thickBot="1">
+      <c r="A30" s="70">
+        <v>17</v>
+      </c>
+      <c r="B30" s="157" t="s">
         <v>206</v>
       </c>
-      <c r="D26" s="148" t="s">
+      <c r="C30" s="68" t="s">
+        <v>237</v>
+      </c>
+      <c r="D30" s="68" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="149" t="s">
+      <c r="E30" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="150"/>
-      <c r="G26" s="151" t="s">
+      <c r="F30" s="159"/>
+      <c r="G30" s="160" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12" thickBot="1">
-      <c r="A27" s="70">
-        <v>14</v>
-      </c>
-      <c r="B27" s="157" t="s">
-        <v>207</v>
-      </c>
-      <c r="C27" s="68" t="s">
-        <v>208</v>
-      </c>
-      <c r="D27" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="158" t="s">
+    <row r="32" spans="1:8" ht="12" thickBot="1">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="173" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="174"/>
+      <c r="E33" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="13">
+      <c r="A34" s="14">
+        <v>1</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="185" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="186"/>
+      <c r="E34" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="159"/>
-      <c r="G27" s="160" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="12" thickBot="1">
-      <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="173" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="174"/>
-      <c r="E30" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="G30" s="35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="13">
-      <c r="A31" s="14">
-        <v>1</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="187" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" s="188"/>
-      <c r="E31" s="46" t="s">
+      <c r="F34" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="46" t="s">
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="1:7" ht="13" customHeight="1">
+      <c r="A35" s="57">
+        <v>2</v>
+      </c>
+      <c r="B35" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="171" t="s">
+        <v>227</v>
+      </c>
+      <c r="D35" s="172"/>
+      <c r="E35" s="52" t="s">
+        <v>235</v>
+      </c>
+      <c r="F35" s="52" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="53" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="13" customHeight="1" thickBot="1">
+      <c r="A36" s="56">
         <v>3</v>
       </c>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="1:8" ht="13" customHeight="1">
-      <c r="A32" s="57">
-        <v>2</v>
-      </c>
-      <c r="B32" s="51" t="s">
-        <v>244</v>
-      </c>
-      <c r="C32" s="192" t="s">
-        <v>237</v>
-      </c>
-      <c r="D32" s="193"/>
-      <c r="E32" s="52" t="s">
-        <v>245</v>
-      </c>
-      <c r="F32" s="52" t="s">
-        <v>245</v>
-      </c>
-      <c r="G32" s="53" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="13" customHeight="1" thickBot="1">
-      <c r="A33" s="56">
-        <v>3</v>
-      </c>
-      <c r="B33" s="54"/>
-      <c r="C33" s="190"/>
-      <c r="D33" s="191"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="55"/>
-    </row>
-    <row r="35" spans="1:7" ht="12" thickBot="1">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="14" thickBot="1">
-      <c r="A36" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="175" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="176"/>
-      <c r="E36" s="175" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" s="189"/>
-      <c r="G36" s="38" t="s">
-        <v>38</v>
-      </c>
+      <c r="B36" s="54"/>
+      <c r="C36" s="169"/>
+      <c r="D36" s="170"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="55"/>
     </row>
     <row r="38" spans="1:7" ht="12" thickBot="1">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14" thickBot="1">
@@ -8215,40 +8339,64 @@
       <c r="B39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="175" t="s">
+      <c r="C39" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="176"/>
-      <c r="E39" s="175" t="s">
+      <c r="D39" s="167"/>
+      <c r="E39" s="166" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="168"/>
+      <c r="G39" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="12" thickBot="1">
+      <c r="A41" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="14" thickBot="1">
+      <c r="A42" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="166" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="167"/>
+      <c r="E42" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="189"/>
-      <c r="G39" s="38" t="s">
+      <c r="F42" s="168"/>
+      <c r="G42" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E39:F39"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -8300,103 +8448,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="167"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="166" t="s">
+      <c r="F2" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="170"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="169"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="168" t="s">
+      <c r="F3" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="172"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="172"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="191" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="169"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="172"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="168" t="s">
+      <c r="C6" s="191" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="169"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="172"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:11" ht="13">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="179"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="180"/>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="182"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="183"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="182"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1">
-      <c r="B10" s="184"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="186"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8639,10 +8787,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="187" t="s">
+      <c r="C25" s="185" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="188"/>
+      <c r="D25" s="186"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -8678,14 +8826,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="175" t="s">
+      <c r="C29" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="176"/>
-      <c r="E29" s="175" t="s">
+      <c r="D29" s="167"/>
+      <c r="E29" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="189"/>
+      <c r="F29" s="168"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -8702,14 +8850,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="175" t="s">
+      <c r="C32" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="176"/>
-      <c r="E32" s="175" t="s">
+      <c r="D32" s="167"/>
+      <c r="E32" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="189"/>
+      <c r="F32" s="168"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -8733,15 +8881,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -8754,6 +8893,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8801,105 +8949,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="167"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="166" t="s">
+      <c r="F2" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="170"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:7" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="169"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="168" t="s">
+      <c r="F3" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="172"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:7" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="172"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:7" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="191" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="169"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="172"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:7" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="168" t="s">
+      <c r="C6" s="191" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="169"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="172"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:7" ht="13">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="179"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="178" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="182"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="183"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="182"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:7" ht="12" thickBot="1">
-      <c r="B10" s="184"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="186"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:7" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9025,10 +9173,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="187" t="s">
+      <c r="C20" s="185" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="188"/>
+      <c r="D20" s="186"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -9064,14 +9212,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="175" t="s">
+      <c r="C24" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="176"/>
-      <c r="E24" s="175" t="s">
+      <c r="D24" s="167"/>
+      <c r="E24" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="189"/>
+      <c r="F24" s="168"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -9088,14 +9236,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="175" t="s">
+      <c r="C27" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="176"/>
-      <c r="E27" s="175" t="s">
+      <c r="D27" s="167"/>
+      <c r="E27" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="189"/>
+      <c r="F27" s="168"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -9113,15 +9261,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -9134,6 +9273,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9181,10 +9329,10 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="167"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
@@ -9197,87 +9345,87 @@
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="169"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="189" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="172"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="172"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="191" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="169"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="172"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="168" t="s">
+      <c r="C6" s="191" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="169"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="172"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:14" ht="13">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="179"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="180"/>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="182"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="183"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="182"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="184"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="186"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -9520,10 +9668,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="187" t="s">
+      <c r="C22" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="188"/>
+      <c r="D22" s="186"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -9543,10 +9691,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="192" t="s">
+      <c r="C23" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="193"/>
+      <c r="D23" s="172"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -9606,14 +9754,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="175" t="s">
+      <c r="C27" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="176"/>
-      <c r="E27" s="175" t="s">
+      <c r="D27" s="167"/>
+      <c r="E27" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="189"/>
+      <c r="F27" s="168"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -9650,14 +9798,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="175" t="s">
+      <c r="C30" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="176"/>
-      <c r="E30" s="175" t="s">
+      <c r="D30" s="167"/>
+      <c r="E30" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="189"/>
+      <c r="F30" s="168"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -9673,14 +9821,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="187" t="s">
+      <c r="C31" s="185" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="188"/>
-      <c r="E31" s="192" t="s">
+      <c r="D31" s="186"/>
+      <c r="E31" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="193"/>
+      <c r="F31" s="172"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -9756,6 +9904,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -9772,14 +9928,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9803,8 +9951,8 @@
   </sheetPr>
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -9834,101 +9982,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="187" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="167"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="166"/>
-      <c r="G2" s="170"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="169"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="189" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="172"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="191" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="172"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="168" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" s="169"/>
+      <c r="C5" s="191" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="172"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="168" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" s="169"/>
+      <c r="C6" s="191" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="172"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="179"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="180"/>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="182"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="183"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="182"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="184"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="186"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9970,22 +10118,22 @@
         <v>143</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="M13" s="128" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="N13" s="128" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="O13" s="128" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="P13" s="128" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="Q13" s="128" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="R13" s="128"/>
       <c r="S13" s="128"/>
@@ -10024,7 +10172,7 @@
         <v>146</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="N14" s="136">
         <v>1</v>
@@ -10070,10 +10218,10 @@
         <v>146</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="N15" s="136">
         <v>1</v>
@@ -10136,7 +10284,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C18" s="65" t="s">
         <v>129</v>
@@ -10199,10 +10347,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>210</v>
+        <v>257</v>
       </c>
       <c r="D21" s="129" t="s">
         <v>148</v>
@@ -10224,7 +10372,7 @@
         <v>134</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
       <c r="D22" s="65" t="s">
         <v>149</v>
@@ -10282,10 +10430,10 @@
       <c r="B27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="187" t="s">
+      <c r="C27" s="185" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="188"/>
+      <c r="D27" s="186"/>
       <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
@@ -10299,20 +10447,20 @@
         <v>2</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="C28" s="192" t="s">
-        <v>238</v>
-      </c>
-      <c r="D28" s="193"/>
+        <v>233</v>
+      </c>
+      <c r="C28" s="171" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" s="172"/>
       <c r="E28" s="52" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="F28" s="52" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G28" s="53" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13" customHeight="1" thickBot="1">
@@ -10320,8 +10468,8 @@
         <v>3</v>
       </c>
       <c r="B29" s="54"/>
-      <c r="C29" s="190"/>
-      <c r="D29" s="191"/>
+      <c r="C29" s="169"/>
+      <c r="D29" s="170"/>
       <c r="E29" s="58"/>
       <c r="F29" s="58"/>
       <c r="G29" s="55"/>
@@ -10338,14 +10486,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="175" t="s">
+      <c r="C32" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="176"/>
-      <c r="E32" s="175" t="s">
+      <c r="D32" s="167"/>
+      <c r="E32" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="189"/>
+      <c r="F32" s="168"/>
       <c r="G32" s="38" t="s">
         <v>38</v>
       </c>
@@ -10355,10 +10503,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="19"/>
-      <c r="C33" s="187" t="s">
+      <c r="C33" s="185" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="188"/>
+      <c r="D33" s="186"/>
       <c r="E33" s="202" t="s">
         <v>151</v>
       </c>
@@ -10379,20 +10527,30 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="175" t="s">
+      <c r="C36" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="176"/>
-      <c r="E36" s="175" t="s">
+      <c r="D36" s="167"/>
+      <c r="E36" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="189"/>
+      <c r="F36" s="168"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -10405,16 +10563,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10438,8 +10586,8 @@
   </sheetPr>
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -10468,101 +10616,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="187" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="167"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="166"/>
-      <c r="G2" s="170"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:18" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="169"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="189" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="172"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:18" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="191" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="168"/>
-      <c r="G4" s="172"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:18" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="168" t="s">
-        <v>222</v>
-      </c>
-      <c r="D5" s="169"/>
+      <c r="C5" s="191" t="s">
+        <v>218</v>
+      </c>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="172"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:18" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="168" t="s">
-        <v>221</v>
-      </c>
-      <c r="D6" s="169"/>
+      <c r="C6" s="191" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="172"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:18" ht="13">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="179"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="180"/>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="182"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="183"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="182"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:18" ht="12" thickBot="1">
-      <c r="B10" s="184"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="186"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:18" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10601,16 +10749,16 @@
         <v>125</v>
       </c>
       <c r="K13" s="128" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="M13" s="128" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="N13" s="128" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="O13" s="128"/>
       <c r="P13" s="128"/>
@@ -10726,10 +10874,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D17" s="129" t="s">
         <v>53</v>
@@ -10749,7 +10897,7 @@
         <v>197</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="D18" s="65" t="s">
         <v>147</v>
@@ -10772,7 +10920,7 @@
         <v>198</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="D19" s="65" t="s">
         <v>147</v>
@@ -10842,10 +10990,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="187" t="s">
+      <c r="C25" s="185" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="188"/>
+      <c r="D25" s="186"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -10859,8 +11007,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="51"/>
-      <c r="C26" s="192"/>
-      <c r="D26" s="193"/>
+      <c r="C26" s="171"/>
+      <c r="D26" s="172"/>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
       <c r="G26" s="20"/>
@@ -10870,8 +11018,8 @@
         <v>3</v>
       </c>
       <c r="B27" s="54"/>
-      <c r="C27" s="190"/>
-      <c r="D27" s="191"/>
+      <c r="C27" s="169"/>
+      <c r="D27" s="170"/>
       <c r="E27" s="58"/>
       <c r="F27" s="58"/>
       <c r="G27" s="55"/>
@@ -10888,14 +11036,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="175" t="s">
+      <c r="C30" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="176"/>
-      <c r="E30" s="175" t="s">
+      <c r="D30" s="167"/>
+      <c r="E30" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="189"/>
+      <c r="F30" s="168"/>
       <c r="G30" s="38" t="s">
         <v>38</v>
       </c>
@@ -10906,7 +11054,7 @@
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="202" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D31" s="203"/>
       <c r="E31" s="206" t="s">
@@ -10923,15 +11071,15 @@
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="204" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D32" s="205"/>
       <c r="E32" s="208" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F32" s="209"/>
       <c r="G32" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" customHeight="1" thickBot="1">
@@ -10939,8 +11087,8 @@
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="190"/>
-      <c r="D33" s="191"/>
+      <c r="C33" s="169"/>
+      <c r="D33" s="170"/>
       <c r="E33" s="210"/>
       <c r="F33" s="211"/>
       <c r="G33" s="55"/>
@@ -10957,26 +11105,28 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="175" t="s">
+      <c r="C36" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="176"/>
-      <c r="E36" s="175" t="s">
+      <c r="D36" s="167"/>
+      <c r="E36" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="176"/>
+      <c r="F36" s="167"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
@@ -10989,14 +11139,12 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>